<commit_message>
Modified my schedule and added new files.
</commit_message>
<xml_diff>
--- a/2019-2020 1st semester.xlsx
+++ b/2019-2020 1st semester.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\MySchedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A994E3A-94A9-43A6-9834-AF5F142735F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650F7D46-1EC6-45DD-AF77-5124DE98D937}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="103">
   <si>
     <t/>
   </si>
@@ -358,6 +358,14 @@
   </si>
   <si>
     <t>CET6</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>答疑</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>网络编程</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -537,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -582,6 +590,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -600,26 +614,32 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -938,18 +958,18 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R35" sqref="R35:R38"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="8" width="6" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="6" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="6" customWidth="1"/>
-    <col min="14" max="17" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="6" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="11" max="13" width="6" hidden="1" customWidth="1"/>
+    <col min="14" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="21" width="6" customWidth="1"/>
     <col min="22" max="22" width="17" customWidth="1"/>
     <col min="23" max="23" width="27" customWidth="1"/>
@@ -959,57 +979,57 @@
       <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
     </row>
     <row r="2" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
       <c r="M2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
     </row>
     <row r="3" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1154,7 +1174,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="18" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1176,7 +1196,7 @@
       <c r="H5" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="21" t="s">
         <v>68</v>
       </c>
       <c r="J5" s="10" t="s">
@@ -1195,12 +1215,12 @@
       <c r="V5" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="W5" s="18" t="s">
+      <c r="W5" s="20" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="9" t="s">
         <v>49</v>
       </c>
@@ -1210,7 +1230,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="21" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="9"/>
@@ -1218,16 +1238,13 @@
       <c r="L6" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="M6" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="O6" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="P6" s="11" t="s">
+      <c r="M6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="O6" s="10" t="s">
         <v>62</v>
       </c>
       <c r="Q6" s="11" t="s">
@@ -1244,10 +1261,10 @@
       <c r="V6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="W6" s="16"/>
+      <c r="W6" s="18"/>
     </row>
     <row r="7" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="9" t="s">
         <v>50</v>
       </c>
@@ -1257,13 +1274,13 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" s="20" t="s">
+      <c r="I7" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="20" t="s">
+      <c r="K7" s="22" t="s">
         <v>96</v>
       </c>
       <c r="L7" s="9"/>
@@ -1277,10 +1294,10 @@
       <c r="T7" s="9"/>
       <c r="U7" s="9"/>
       <c r="V7" s="9"/>
-      <c r="W7" s="16"/>
+      <c r="W7" s="18"/>
     </row>
     <row r="8" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="9" t="s">
         <v>51</v>
       </c>
@@ -1290,30 +1307,35 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="20" t="s">
+      <c r="I8" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="22" t="s">
         <v>96</v>
       </c>
       <c r="M8" s="22" t="s">
         <v>96</v>
       </c>
       <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
+      <c r="O8" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q8" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="R8" s="29" t="s">
+        <v>98</v>
+      </c>
       <c r="S8" s="9"/>
       <c r="T8" s="9"/>
       <c r="U8" s="9"/>
       <c r="V8" s="9"/>
-      <c r="W8" s="16"/>
+      <c r="W8" s="18"/>
     </row>
     <row r="9" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="9" t="s">
         <v>52</v>
       </c>
@@ -1323,30 +1345,30 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="21" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>92</v>
       </c>
       <c r="K9" s="9"/>
-      <c r="L9" s="21"/>
+      <c r="L9" s="23"/>
       <c r="M9" s="23"/>
       <c r="N9" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
       <c r="S9" s="9"/>
       <c r="T9" s="9"/>
       <c r="U9" s="9"/>
       <c r="V9" s="9"/>
-      <c r="W9" s="16"/>
+      <c r="W9" s="18"/>
     </row>
     <row r="10" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="9" t="s">
         <v>53</v>
       </c>
@@ -1356,7 +1378,7 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="21" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="9"/>
@@ -1372,10 +1394,10 @@
       <c r="T10" s="9"/>
       <c r="U10" s="9"/>
       <c r="V10" s="9"/>
-      <c r="W10" s="16"/>
+      <c r="W10" s="18"/>
     </row>
     <row r="11" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="18" t="s">
         <v>54</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1393,7 +1415,7 @@
       <c r="G11" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="19" t="s">
+      <c r="H11" s="21" t="s">
         <v>68</v>
       </c>
       <c r="I11" s="10" t="s">
@@ -1408,7 +1430,7 @@
       <c r="L11" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="10" t="s">
         <v>62</v>
       </c>
       <c r="N11" s="14"/>
@@ -1422,10 +1444,10 @@
       <c r="V11" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="W11" s="16"/>
+      <c r="W11" s="18"/>
     </row>
     <row r="12" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="16"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="9" t="s">
         <v>49</v>
       </c>
@@ -1434,7 +1456,7 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="19" t="s">
+      <c r="H12" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I12" s="9"/>
@@ -1451,10 +1473,10 @@
       <c r="T12" s="9"/>
       <c r="U12" s="9"/>
       <c r="V12" s="9"/>
-      <c r="W12" s="16"/>
+      <c r="W12" s="18"/>
     </row>
     <row r="13" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="9" t="s">
         <v>50</v>
       </c>
@@ -1471,7 +1493,7 @@
       <c r="G13" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I13" s="10" t="s">
@@ -1486,7 +1508,7 @@
       <c r="L13" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="M13" s="11" t="s">
+      <c r="M13" s="10" t="s">
         <v>62</v>
       </c>
       <c r="N13" s="22" t="s">
@@ -1498,42 +1520,44 @@
       <c r="P13" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="Q13" s="22" t="s">
+      <c r="Q13" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="R13" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="R13" s="9"/>
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
       <c r="U13" s="9"/>
       <c r="V13" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="W13" s="16"/>
+      <c r="W13" s="18"/>
     </row>
     <row r="14" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
+      <c r="A14" s="18"/>
       <c r="B14" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="22" t="s">
         <v>81</v>
       </c>
       <c r="F14" s="15"/>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="H14" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" s="20" t="s">
+      <c r="H14" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="J14" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="K14" s="20" t="s">
+      <c r="K14" s="22" t="s">
         <v>87</v>
       </c>
       <c r="M14" s="22" t="s">
@@ -1542,31 +1566,31 @@
       <c r="N14" s="23"/>
       <c r="O14" s="23"/>
       <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="9"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="30"/>
       <c r="S14" s="9"/>
       <c r="T14" s="9"/>
       <c r="U14" s="9"/>
       <c r="V14" s="9"/>
-      <c r="W14" s="16"/>
+      <c r="W14" s="18"/>
     </row>
     <row r="15" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="16"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="21"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="20" t="s">
+      <c r="G15" s="23"/>
+      <c r="H15" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="22" t="s">
         <v>88</v>
       </c>
       <c r="M15" s="23"/>
@@ -1581,10 +1605,10 @@
       <c r="T15" s="9"/>
       <c r="U15" s="9"/>
       <c r="V15" s="9"/>
-      <c r="W15" s="16"/>
+      <c r="W15" s="18"/>
     </row>
     <row r="16" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="9" t="s">
         <v>53</v>
       </c>
@@ -1593,13 +1617,13 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="19" t="s">
+      <c r="H16" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-      <c r="L16" s="21"/>
+      <c r="L16" s="23"/>
       <c r="M16" s="9"/>
       <c r="N16" s="23"/>
       <c r="O16" s="9"/>
@@ -1610,10 +1634,10 @@
       <c r="T16" s="9"/>
       <c r="U16" s="9"/>
       <c r="V16" s="9"/>
-      <c r="W16" s="16"/>
+      <c r="W16" s="18"/>
     </row>
     <row r="17" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="18" t="s">
         <v>55</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -1624,7 +1648,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I17" s="9"/>
@@ -1639,14 +1663,14 @@
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
-      <c r="U17" s="19" t="s">
+      <c r="U17" s="21" t="s">
         <v>66</v>
       </c>
       <c r="V17" s="9"/>
-      <c r="W17" s="16"/>
+      <c r="W17" s="18"/>
     </row>
     <row r="18" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="9" t="s">
         <v>49</v>
       </c>
@@ -1665,7 +1689,7 @@
       <c r="G18" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I18" s="10" t="s">
@@ -1684,16 +1708,16 @@
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
       <c r="T18" s="9"/>
-      <c r="U18" s="19" t="s">
+      <c r="U18" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V18" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="W18" s="16"/>
+      <c r="W18" s="18"/>
     </row>
     <row r="19" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="9" t="s">
         <v>50</v>
       </c>
@@ -1712,7 +1736,7 @@
       <c r="G19" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I19" s="10" t="s">
@@ -1724,37 +1748,31 @@
       <c r="K19" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="L19" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="M19" s="11" t="s">
+      <c r="L19" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M19" s="10" t="s">
         <v>62</v>
       </c>
       <c r="N19" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="O19" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="P19" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q19" s="22" t="s">
-        <v>98</v>
-      </c>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
       <c r="T19" s="9"/>
-      <c r="U19" s="19" t="s">
+      <c r="U19" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V19" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="W19" s="16"/>
+      <c r="W19" s="18"/>
     </row>
     <row r="20" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="16"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="9" t="s">
         <v>51</v>
       </c>
@@ -1773,7 +1791,7 @@
       <c r="G20" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="H20" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I20" s="10" t="s">
@@ -1785,53 +1803,55 @@
       <c r="K20" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="L20" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="M20" s="11" t="s">
+      <c r="L20" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M20" s="10" t="s">
         <v>62</v>
       </c>
       <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="11" t="s">
+        <v>79</v>
+      </c>
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
-      <c r="U20" s="19" t="s">
+      <c r="U20" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V20" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="W20" s="16"/>
+      <c r="W20" s="18"/>
     </row>
     <row r="21" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="16"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="H21" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I21" s="20" t="s">
+      <c r="H21" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="J21" s="20" t="s">
+      <c r="J21" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="K21" s="20" t="s">
+      <c r="K21" s="22" t="s">
         <v>89</v>
       </c>
       <c r="L21" s="22" t="s">
@@ -1847,28 +1867,28 @@
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
       <c r="T21" s="9"/>
-      <c r="U21" s="19" t="s">
+      <c r="U21" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V21" s="9"/>
-      <c r="W21" s="16"/>
+      <c r="W21" s="18"/>
     </row>
     <row r="22" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="16"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
       <c r="L22" s="23"/>
       <c r="M22" s="9"/>
       <c r="N22" s="23"/>
@@ -1878,14 +1898,14 @@
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
       <c r="T22" s="9"/>
-      <c r="U22" s="19" t="s">
+      <c r="U22" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V22" s="9"/>
-      <c r="W22" s="16"/>
+      <c r="W22" s="18"/>
     </row>
     <row r="23" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="18" t="s">
         <v>56</v>
       </c>
       <c r="B23" s="9" t="s">
@@ -1896,7 +1916,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I23" s="9"/>
@@ -1913,14 +1933,14 @@
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
       <c r="T23" s="9"/>
-      <c r="U23" s="19" t="s">
+      <c r="U23" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V23" s="9"/>
-      <c r="W23" s="16"/>
+      <c r="W23" s="18"/>
     </row>
     <row r="24" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="9" t="s">
         <v>49</v>
       </c>
@@ -1929,7 +1949,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="19" t="s">
+      <c r="H24" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I24" s="9"/>
@@ -1944,30 +1964,30 @@
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
-      <c r="U24" s="19" t="s">
+      <c r="U24" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V24" s="9"/>
-      <c r="W24" s="16"/>
+      <c r="W24" s="18"/>
     </row>
     <row r="25" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="16"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="12"/>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G25" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="H25" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I25" s="20" t="s">
+      <c r="H25" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" s="22" t="s">
         <v>86</v>
       </c>
       <c r="J25" s="9"/>
@@ -1981,26 +2001,26 @@
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
-      <c r="U25" s="19" t="s">
+      <c r="U25" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V25" s="9"/>
-      <c r="W25" s="16"/>
+      <c r="W25" s="18"/>
     </row>
     <row r="26" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="12"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I26" s="21"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" s="23"/>
       <c r="J26" s="10" t="s">
         <v>94</v>
       </c>
@@ -2018,14 +2038,14 @@
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
       <c r="T26" s="9"/>
-      <c r="U26" s="19" t="s">
+      <c r="U26" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V26" s="9"/>
-      <c r="W26" s="16"/>
+      <c r="W26" s="18"/>
     </row>
     <row r="27" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="16"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="9" t="s">
         <v>52</v>
       </c>
@@ -2034,7 +2054,7 @@
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="19" t="s">
+      <c r="H27" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I27" s="10" t="s">
@@ -2053,14 +2073,14 @@
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
-      <c r="U27" s="19" t="s">
+      <c r="U27" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V27" s="9"/>
-      <c r="W27" s="16"/>
+      <c r="W27" s="18"/>
     </row>
     <row r="28" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="16"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="9" t="s">
         <v>53</v>
       </c>
@@ -2069,7 +2089,7 @@
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="19" t="s">
+      <c r="H28" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I28" s="9"/>
@@ -2084,14 +2104,14 @@
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
       <c r="T28" s="9"/>
-      <c r="U28" s="19" t="s">
+      <c r="U28" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V28" s="9"/>
-      <c r="W28" s="16"/>
+      <c r="W28" s="18"/>
     </row>
     <row r="29" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="18" t="s">
         <v>57</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -2099,12 +2119,12 @@
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="21" t="s">
         <v>67</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="19" t="s">
+      <c r="H29" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I29" s="9"/>
@@ -2113,46 +2133,48 @@
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
+      <c r="O29" s="10" t="s">
+        <v>101</v>
+      </c>
       <c r="P29" s="9"/>
       <c r="Q29" s="9"/>
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
       <c r="T29" s="9"/>
-      <c r="U29" s="19" t="s">
+      <c r="U29" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V29" s="9"/>
-      <c r="W29" s="16"/>
+      <c r="W29" s="18"/>
     </row>
     <row r="30" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="16"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="19" t="s">
+      <c r="H30" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
-      <c r="L30" s="11" t="s">
+      <c r="L30" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="M30" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="N30" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="O30" s="11" t="s">
+      <c r="M30" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="N30" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="O30" s="10" t="s">
         <v>62</v>
       </c>
       <c r="P30" s="11" t="s">
@@ -2168,16 +2190,16 @@
         <v>62</v>
       </c>
       <c r="T30" s="9"/>
-      <c r="U30" s="19" t="s">
+      <c r="U30" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V30" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="W30" s="16"/>
+      <c r="W30" s="18"/>
     </row>
     <row r="31" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="16"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="9" t="s">
         <v>50</v>
       </c>
@@ -2187,7 +2209,7 @@
       <c r="D31" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F31" s="10" t="s">
@@ -2196,7 +2218,7 @@
       <c r="G31" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H31" s="19" t="s">
+      <c r="H31" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I31" s="10" t="s">
@@ -2208,10 +2230,10 @@
       <c r="K31" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="L31" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="M31" s="11" t="s">
+      <c r="L31" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M31" s="10" t="s">
         <v>62</v>
       </c>
       <c r="N31" s="9"/>
@@ -2221,16 +2243,16 @@
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
       <c r="T31" s="9"/>
-      <c r="U31" s="19" t="s">
+      <c r="U31" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V31" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="W31" s="16"/>
+      <c r="W31" s="18"/>
     </row>
     <row r="32" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="16"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="9" t="s">
         <v>51</v>
       </c>
@@ -2240,7 +2262,7 @@
       <c r="D32" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E32" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F32" s="10" t="s">
@@ -2249,7 +2271,7 @@
       <c r="G32" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H32" s="19" t="s">
+      <c r="H32" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I32" s="10" t="s">
@@ -2261,10 +2283,10 @@
       <c r="K32" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="L32" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="M32" s="11" t="s">
+      <c r="L32" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M32" s="10" t="s">
         <v>62</v>
       </c>
       <c r="N32" s="9"/>
@@ -2274,27 +2296,27 @@
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
       <c r="T32" s="9"/>
-      <c r="U32" s="19" t="s">
+      <c r="U32" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V32" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="W32" s="16"/>
+      <c r="W32" s="18"/>
     </row>
     <row r="33" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="16"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="19" t="s">
+      <c r="H33" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I33" s="9"/>
@@ -2309,25 +2331,25 @@
       <c r="R33" s="9"/>
       <c r="S33" s="9"/>
       <c r="T33" s="9"/>
-      <c r="U33" s="19" t="s">
+      <c r="U33" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V33" s="9"/>
-      <c r="W33" s="16"/>
+      <c r="W33" s="18"/>
     </row>
     <row r="34" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="16"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="19" t="s">
+      <c r="H34" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I34" s="9"/>
@@ -2342,14 +2364,14 @@
       <c r="R34" s="9"/>
       <c r="S34" s="9"/>
       <c r="T34" s="9"/>
-      <c r="U34" s="19" t="s">
+      <c r="U34" s="21" t="s">
         <v>0</v>
       </c>
       <c r="V34" s="9"/>
-      <c r="W34" s="16"/>
+      <c r="W34" s="18"/>
     </row>
     <row r="35" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="18" t="s">
         <v>58</v>
       </c>
       <c r="B35" s="9" t="s">
@@ -2357,19 +2379,19 @@
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
-      <c r="H35" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I35" s="20" t="s">
+      <c r="H35" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I35" s="22" t="s">
         <v>97</v>
       </c>
       <c r="J35" s="9"/>
-      <c r="K35" s="20" t="s">
+      <c r="K35" s="22" t="s">
         <v>97</v>
       </c>
       <c r="L35" s="9"/>
@@ -2385,26 +2407,26 @@
       <c r="T35" s="9"/>
       <c r="U35" s="9"/>
       <c r="V35" s="9"/>
-      <c r="W35" s="16"/>
+      <c r="W35" s="18"/>
     </row>
     <row r="36" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="16"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
-      <c r="H36" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I36" s="21"/>
+      <c r="H36" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I36" s="23"/>
       <c r="J36" s="9"/>
-      <c r="K36" s="21"/>
+      <c r="K36" s="23"/>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
@@ -2416,28 +2438,28 @@
       <c r="T36" s="9"/>
       <c r="U36" s="9"/>
       <c r="V36" s="9"/>
-      <c r="W36" s="16"/>
+      <c r="W36" s="18"/>
     </row>
     <row r="37" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="16"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
-      <c r="H37" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I37" s="20" t="s">
+      <c r="H37" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" s="22" t="s">
         <v>95</v>
       </c>
       <c r="J37" s="9"/>
-      <c r="K37" s="20" t="s">
+      <c r="K37" s="22" t="s">
         <v>95</v>
       </c>
       <c r="L37" s="9"/>
@@ -2453,26 +2475,26 @@
       <c r="T37" s="9"/>
       <c r="U37" s="9"/>
       <c r="V37" s="9"/>
-      <c r="W37" s="16"/>
+      <c r="W37" s="18"/>
     </row>
     <row r="38" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="16"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
-      <c r="H38" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="I38" s="21"/>
+      <c r="H38" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="I38" s="23"/>
       <c r="J38" s="9"/>
-      <c r="K38" s="21"/>
+      <c r="K38" s="23"/>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
@@ -2484,21 +2506,21 @@
       <c r="T38" s="9"/>
       <c r="U38" s="9"/>
       <c r="V38" s="9"/>
-      <c r="W38" s="16"/>
+      <c r="W38" s="18"/>
     </row>
     <row r="39" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="16"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
-      <c r="H39" s="19" t="s">
+      <c r="H39" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I39" s="9"/>
@@ -2515,21 +2537,21 @@
       <c r="T39" s="9"/>
       <c r="U39" s="9"/>
       <c r="V39" s="9"/>
-      <c r="W39" s="16"/>
+      <c r="W39" s="18"/>
     </row>
     <row r="40" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="16"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
-      <c r="H40" s="19" t="s">
+      <c r="H40" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I40" s="9"/>
@@ -2546,10 +2568,10 @@
       <c r="T40" s="9"/>
       <c r="U40" s="9"/>
       <c r="V40" s="9"/>
-      <c r="W40" s="16"/>
+      <c r="W40" s="18"/>
     </row>
     <row r="41" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="18" t="s">
         <v>59</v>
       </c>
       <c r="B41" s="9" t="s">
@@ -2557,12 +2579,12 @@
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
-      <c r="H41" s="19" t="s">
+      <c r="H41" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I41" s="9"/>
@@ -2581,21 +2603,21 @@
       <c r="V41" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="W41" s="16"/>
+      <c r="W41" s="18"/>
     </row>
     <row r="42" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="16"/>
+      <c r="A42" s="18"/>
       <c r="B42" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
-      <c r="E42" s="19" t="s">
+      <c r="E42" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
-      <c r="H42" s="19" t="s">
+      <c r="H42" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I42" s="9"/>
@@ -2614,21 +2636,21 @@
       <c r="V42" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="W42" s="16"/>
+      <c r="W42" s="18"/>
     </row>
     <row r="43" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="16"/>
+      <c r="A43" s="18"/>
       <c r="B43" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
-      <c r="E43" s="19" t="s">
+      <c r="E43" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
-      <c r="H43" s="19" t="s">
+      <c r="H43" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I43" s="9"/>
@@ -2647,21 +2669,21 @@
       <c r="V43" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="W43" s="16"/>
+      <c r="W43" s="18"/>
     </row>
     <row r="44" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="16"/>
+      <c r="A44" s="18"/>
       <c r="B44" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
-      <c r="E44" s="19" t="s">
+      <c r="E44" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
-      <c r="H44" s="19" t="s">
+      <c r="H44" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I44" s="9"/>
@@ -2680,21 +2702,21 @@
       <c r="V44" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="W44" s="16"/>
+      <c r="W44" s="18"/>
     </row>
     <row r="45" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="16"/>
+      <c r="A45" s="18"/>
       <c r="B45" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
-      <c r="E45" s="19" t="s">
+      <c r="E45" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
-      <c r="H45" s="19" t="s">
+      <c r="H45" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I45" s="9"/>
@@ -2713,21 +2735,21 @@
       <c r="V45" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="W45" s="16"/>
+      <c r="W45" s="18"/>
     </row>
     <row r="46" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="16"/>
+      <c r="A46" s="18"/>
       <c r="B46" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
-      <c r="E46" s="19" t="s">
+      <c r="E46" s="21" t="s">
         <v>0</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
-      <c r="H46" s="19" t="s">
+      <c r="H46" s="21" t="s">
         <v>0</v>
       </c>
       <c r="I46" s="9"/>
@@ -2744,50 +2766,51 @@
       <c r="T46" s="9"/>
       <c r="U46" s="9"/>
       <c r="V46" s="9"/>
-      <c r="W46" s="16"/>
+      <c r="W46" s="18"/>
     </row>
     <row r="47" spans="1:23" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="16"/>
-      <c r="H47" s="16"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="16"/>
-      <c r="K47" s="16"/>
-      <c r="L47" s="16"/>
-      <c r="M47" s="16"/>
-      <c r="N47" s="16"/>
-      <c r="O47" s="16"/>
-      <c r="P47" s="16"/>
-      <c r="Q47" s="16"/>
-      <c r="R47" s="16"/>
-      <c r="S47" s="16"/>
-      <c r="T47" s="16"/>
-      <c r="U47" s="16"/>
-      <c r="V47" s="16"/>
-      <c r="W47" s="16"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
+      <c r="T47" s="18"/>
+      <c r="U47" s="18"/>
+      <c r="V47" s="18"/>
+      <c r="W47" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="56">
+  <mergeCells count="57">
     <mergeCell ref="R35:R36"/>
     <mergeCell ref="R37:R38"/>
     <mergeCell ref="N9:N10"/>
     <mergeCell ref="N13:N14"/>
     <mergeCell ref="M26:M27"/>
     <mergeCell ref="N19:N20"/>
-    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="O13:O14"/>
     <mergeCell ref="P13:P14"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="N21:N22"/>
     <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="N21:N22"/>
     <mergeCell ref="I37:I38"/>
     <mergeCell ref="K37:K38"/>
     <mergeCell ref="I35:I36"/>

</xml_diff>

<commit_message>
Modified my schedule and added next semester schedule.
</commit_message>
<xml_diff>
--- a/2019-2020 1st semester.xlsx
+++ b/2019-2020 1st semester.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\MySchedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650F7D46-1EC6-45DD-AF77-5124DE98D937}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E84D93-365C-4B2A-8759-504C4B91489E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="106">
   <si>
     <t/>
   </si>
@@ -366,6 +366,18 @@
   </si>
   <si>
     <t>网络编程</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>主北2</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1南308</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>DZZH</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -477,7 +489,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -541,11 +553,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -596,9 +619,39 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -608,38 +661,20 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -958,7 +993,7 @@
   <dimension ref="A1:W47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="V41" sqref="V41:V45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -970,66 +1005,68 @@
     <col min="11" max="13" width="6" hidden="1" customWidth="1"/>
     <col min="14" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="6" customWidth="1"/>
+    <col min="18" max="18" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="6" customWidth="1"/>
+    <col min="21" max="21" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17" customWidth="1"/>
     <col min="23" max="23" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
     </row>
     <row r="2" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="26" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="18"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
     </row>
     <row r="3" spans="1:23" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1174,7 +1211,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="26" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1196,7 +1233,7 @@
       <c r="H5" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="31" t="s">
         <v>68</v>
       </c>
       <c r="J5" s="10" t="s">
@@ -1208,19 +1245,22 @@
       <c r="O5" s="9"/>
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
+      <c r="R5" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
+      <c r="U5" s="32" t="s">
+        <v>103</v>
+      </c>
       <c r="V5" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="W5" s="20" t="s">
+      <c r="W5" s="30" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="9" t="s">
         <v>49</v>
       </c>
@@ -1230,7 +1270,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="31" t="s">
         <v>0</v>
       </c>
       <c r="J6" s="9"/>
@@ -1247,24 +1287,24 @@
       <c r="O6" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="Q6" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="R6" s="11" t="s">
+      <c r="Q6" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="10" t="s">
         <v>62</v>
       </c>
       <c r="S6" s="11" t="s">
         <v>62</v>
       </c>
       <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
+      <c r="U6" s="33"/>
       <c r="V6" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="W6" s="18"/>
+      <c r="W6" s="26"/>
     </row>
     <row r="7" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="9" t="s">
         <v>50</v>
       </c>
@@ -1274,13 +1314,13 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" s="22" t="s">
+      <c r="I7" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="K7" s="21" t="s">
         <v>96</v>
       </c>
       <c r="L7" s="9"/>
@@ -1289,15 +1329,17 @@
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
+      <c r="R7" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="S7" s="9"/>
       <c r="T7" s="9"/>
       <c r="U7" s="9"/>
       <c r="V7" s="9"/>
-      <c r="W7" s="18"/>
+      <c r="W7" s="26"/>
     </row>
     <row r="8" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="9" t="s">
         <v>51</v>
       </c>
@@ -1307,35 +1349,37 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="22" t="s">
+      <c r="I8" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="M8" s="22" t="s">
+      <c r="M8" s="21" t="s">
         <v>96</v>
       </c>
       <c r="N8" s="9"/>
-      <c r="O8" s="22" t="s">
+      <c r="O8" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="Q8" s="29" t="s">
+      <c r="Q8" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="R8" s="29" t="s">
+      <c r="R8" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="S8" s="9"/>
+      <c r="S8" s="20" t="s">
+        <v>105</v>
+      </c>
       <c r="T8" s="9"/>
       <c r="U8" s="9"/>
       <c r="V8" s="9"/>
-      <c r="W8" s="18"/>
+      <c r="W8" s="26"/>
     </row>
     <row r="9" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="9" t="s">
         <v>52</v>
       </c>
@@ -1345,30 +1389,32 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="31" t="s">
         <v>0</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>92</v>
       </c>
       <c r="K9" s="9"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="22" t="s">
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="O9" s="23"/>
+      <c r="O9" s="22"/>
       <c r="P9" s="17"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="9"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="20" t="s">
+        <v>105</v>
+      </c>
       <c r="T9" s="9"/>
       <c r="U9" s="9"/>
       <c r="V9" s="9"/>
-      <c r="W9" s="18"/>
+      <c r="W9" s="26"/>
     </row>
     <row r="10" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="9" t="s">
         <v>53</v>
       </c>
@@ -1378,26 +1424,28 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="31" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="23"/>
+      <c r="N10" s="22"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
       <c r="Q10" s="9"/>
       <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
+      <c r="S10" s="20" t="s">
+        <v>105</v>
+      </c>
       <c r="T10" s="9"/>
       <c r="U10" s="9"/>
       <c r="V10" s="9"/>
-      <c r="W10" s="18"/>
+      <c r="W10" s="26"/>
     </row>
     <row r="11" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="26" t="s">
         <v>54</v>
       </c>
       <c r="B11" s="9" t="s">
@@ -1415,7 +1463,7 @@
       <c r="G11" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="31" t="s">
         <v>68</v>
       </c>
       <c r="I11" s="10" t="s">
@@ -1437,17 +1485,18 @@
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
+      <c r="R11" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="T11" s="9"/>
       <c r="U11" s="9"/>
       <c r="V11" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="W11" s="18"/>
+      <c r="W11" s="26"/>
     </row>
     <row r="12" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="9" t="s">
         <v>49</v>
       </c>
@@ -1456,7 +1505,7 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I12" s="9"/>
@@ -1468,15 +1517,17 @@
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
       <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
+      <c r="R12" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="S12" s="9"/>
       <c r="T12" s="9"/>
       <c r="U12" s="9"/>
       <c r="V12" s="9"/>
-      <c r="W12" s="18"/>
+      <c r="W12" s="26"/>
     </row>
     <row r="13" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="9" t="s">
         <v>50</v>
       </c>
@@ -1493,7 +1544,7 @@
       <c r="G13" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I13" s="10" t="s">
@@ -1511,90 +1562,94 @@
       <c r="M13" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="N13" s="22" t="s">
+      <c r="N13" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="O13" s="22" t="s">
+      <c r="O13" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="P13" s="22" t="s">
+      <c r="P13" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="Q13" s="31" t="s">
+      <c r="Q13" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="R13" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="S13" s="9"/>
+      <c r="R13" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="S13" s="20" t="s">
+        <v>105</v>
+      </c>
       <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
+      <c r="U13" s="18"/>
       <c r="V13" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="W13" s="18"/>
+      <c r="W13" s="26"/>
     </row>
     <row r="14" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="21" t="s">
         <v>81</v>
       </c>
       <c r="F14" s="15"/>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="H14" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" s="22" t="s">
+      <c r="H14" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="J14" s="22" t="s">
+      <c r="J14" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K14" s="22" t="s">
+      <c r="K14" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="M14" s="22" t="s">
+      <c r="M14" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="9"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="24"/>
+      <c r="S14" s="20" t="s">
+        <v>105</v>
+      </c>
       <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
+      <c r="U14" s="18"/>
       <c r="V14" s="9"/>
-      <c r="W14" s="18"/>
+      <c r="W14" s="26"/>
     </row>
     <row r="15" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="23"/>
+      <c r="E15" s="22"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="22" t="s">
+      <c r="G15" s="22"/>
+      <c r="H15" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="M15" s="23"/>
-      <c r="N15" s="22" t="s">
+      <c r="M15" s="22"/>
+      <c r="N15" s="21" t="s">
         <v>89</v>
       </c>
       <c r="O15" s="9"/>
@@ -1605,10 +1660,10 @@
       <c r="T15" s="9"/>
       <c r="U15" s="9"/>
       <c r="V15" s="9"/>
-      <c r="W15" s="18"/>
+      <c r="W15" s="26"/>
     </row>
     <row r="16" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="9" t="s">
         <v>53</v>
       </c>
@@ -1617,15 +1672,15 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-      <c r="L16" s="23"/>
+      <c r="L16" s="22"/>
       <c r="M16" s="9"/>
-      <c r="N16" s="23"/>
+      <c r="N16" s="22"/>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
@@ -1634,10 +1689,10 @@
       <c r="T16" s="9"/>
       <c r="U16" s="9"/>
       <c r="V16" s="9"/>
-      <c r="W16" s="18"/>
+      <c r="W16" s="26"/>
     </row>
     <row r="17" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="26" t="s">
         <v>55</v>
       </c>
       <c r="B17" s="9" t="s">
@@ -1648,7 +1703,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="21" t="s">
+      <c r="H17" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I17" s="9"/>
@@ -1663,14 +1718,14 @@
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
-      <c r="U17" s="21" t="s">
+      <c r="U17" s="34" t="s">
         <v>66</v>
       </c>
       <c r="V17" s="9"/>
-      <c r="W17" s="18"/>
+      <c r="W17" s="26"/>
     </row>
     <row r="18" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
+      <c r="A18" s="26"/>
       <c r="B18" s="9" t="s">
         <v>49</v>
       </c>
@@ -1689,7 +1744,7 @@
       <c r="G18" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I18" s="10" t="s">
@@ -1705,19 +1760,17 @@
       <c r="O18" s="9"/>
       <c r="P18" s="9"/>
       <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
+      <c r="R18" s="13"/>
       <c r="S18" s="9"/>
       <c r="T18" s="9"/>
-      <c r="U18" s="21" t="s">
-        <v>0</v>
-      </c>
+      <c r="U18" s="35"/>
       <c r="V18" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="W18" s="18"/>
+      <c r="W18" s="26"/>
     </row>
     <row r="19" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="9" t="s">
         <v>50</v>
       </c>
@@ -1736,7 +1789,7 @@
       <c r="G19" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="H19" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I19" s="10" t="s">
@@ -1754,25 +1807,25 @@
       <c r="M19" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="N19" s="22" t="s">
+      <c r="N19" s="21" t="s">
         <v>98</v>
       </c>
       <c r="O19" s="16"/>
       <c r="P19" s="16"/>
       <c r="Q19" s="16"/>
-      <c r="R19" s="9"/>
+      <c r="R19" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="S19" s="9"/>
       <c r="T19" s="9"/>
-      <c r="U19" s="21" t="s">
-        <v>0</v>
-      </c>
+      <c r="U19" s="35"/>
       <c r="V19" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="W19" s="18"/>
+      <c r="W19" s="26"/>
     </row>
     <row r="20" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="9" t="s">
         <v>51</v>
       </c>
@@ -1791,7 +1844,7 @@
       <c r="G20" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H20" s="21" t="s">
+      <c r="H20" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I20" s="10" t="s">
@@ -1809,103 +1862,105 @@
       <c r="M20" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="N20" s="23"/>
+      <c r="N20" s="22"/>
       <c r="O20" s="16"/>
       <c r="P20" s="16"/>
-      <c r="Q20" s="11" t="s">
+      <c r="Q20" s="10" t="s">
         <v>79</v>
       </c>
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
-      <c r="U20" s="21" t="s">
-        <v>0</v>
-      </c>
+      <c r="U20" s="35"/>
       <c r="V20" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="W20" s="18"/>
+      <c r="W20" s="26"/>
     </row>
     <row r="21" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="18"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="G21" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="H21" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="I21" s="22" t="s">
+      <c r="H21" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="J21" s="22" t="s">
+      <c r="J21" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="K21" s="22" t="s">
+      <c r="K21" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="L21" s="22" t="s">
+      <c r="L21" s="21" t="s">
         <v>95</v>
       </c>
       <c r="M21" s="9"/>
-      <c r="N21" s="22" t="s">
+      <c r="N21" s="21" t="s">
         <v>88</v>
       </c>
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
+      <c r="Q21" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="R21" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="S21" s="9"/>
       <c r="T21" s="9"/>
-      <c r="U21" s="21" t="s">
-        <v>0</v>
-      </c>
+      <c r="U21" s="36"/>
       <c r="V21" s="9"/>
-      <c r="W21" s="18"/>
+      <c r="W21" s="26"/>
     </row>
     <row r="22" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="18"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
       <c r="M22" s="9"/>
-      <c r="N22" s="23"/>
+      <c r="N22" s="22"/>
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="S22" s="9"/>
       <c r="T22" s="9"/>
-      <c r="U22" s="21" t="s">
+      <c r="U22" s="19" t="s">
         <v>0</v>
       </c>
       <c r="V22" s="9"/>
-      <c r="W22" s="18"/>
+      <c r="W22" s="26"/>
     </row>
     <row r="23" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="26" t="s">
         <v>56</v>
       </c>
       <c r="B23" s="9" t="s">
@@ -1916,7 +1971,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="21" t="s">
+      <c r="H23" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I23" s="9"/>
@@ -1930,17 +1985,19 @@
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
       <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
+      <c r="R23" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="S23" s="9"/>
       <c r="T23" s="9"/>
-      <c r="U23" s="21" t="s">
+      <c r="U23" s="19" t="s">
         <v>0</v>
       </c>
       <c r="V23" s="9"/>
-      <c r="W23" s="18"/>
+      <c r="W23" s="26"/>
     </row>
     <row r="24" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
+      <c r="A24" s="26"/>
       <c r="B24" s="9" t="s">
         <v>49</v>
       </c>
@@ -1949,7 +2006,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="21" t="s">
+      <c r="H24" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I24" s="9"/>
@@ -1961,33 +2018,35 @@
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
       <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
+      <c r="R24" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
-      <c r="U24" s="21" t="s">
+      <c r="U24" s="19" t="s">
         <v>0</v>
       </c>
       <c r="V24" s="9"/>
-      <c r="W24" s="18"/>
+      <c r="W24" s="26"/>
     </row>
     <row r="25" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="18"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="12"/>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="H25" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="I25" s="22" t="s">
+      <c r="H25" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" s="21" t="s">
         <v>86</v>
       </c>
       <c r="J25" s="9"/>
@@ -2001,34 +2060,34 @@
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
       <c r="T25" s="9"/>
-      <c r="U25" s="21" t="s">
-        <v>0</v>
+      <c r="U25" s="32" t="s">
+        <v>104</v>
       </c>
       <c r="V25" s="9"/>
-      <c r="W25" s="18"/>
+      <c r="W25" s="26"/>
     </row>
     <row r="26" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="18"/>
+      <c r="A26" s="26"/>
       <c r="B26" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="12"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="I26" s="23"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" s="22"/>
       <c r="J26" s="10" t="s">
         <v>94</v>
       </c>
       <c r="K26" s="9"/>
-      <c r="L26" s="22" t="s">
+      <c r="L26" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="M26" s="22" t="s">
+      <c r="M26" s="21" t="s">
         <v>97</v>
       </c>
       <c r="N26" s="9"/>
@@ -2038,14 +2097,12 @@
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
       <c r="T26" s="9"/>
-      <c r="U26" s="21" t="s">
-        <v>0</v>
-      </c>
+      <c r="U26" s="33"/>
       <c r="V26" s="9"/>
-      <c r="W26" s="18"/>
+      <c r="W26" s="26"/>
     </row>
     <row r="27" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="18"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="9" t="s">
         <v>52</v>
       </c>
@@ -2054,7 +2111,7 @@
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="21" t="s">
+      <c r="H27" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I27" s="10" t="s">
@@ -2064,8 +2121,8 @@
         <v>94</v>
       </c>
       <c r="K27" s="9"/>
-      <c r="L27" s="23"/>
-      <c r="M27" s="23"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
@@ -2073,14 +2130,14 @@
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
       <c r="T27" s="9"/>
-      <c r="U27" s="21" t="s">
+      <c r="U27" s="19" t="s">
         <v>0</v>
       </c>
       <c r="V27" s="9"/>
-      <c r="W27" s="18"/>
+      <c r="W27" s="26"/>
     </row>
     <row r="28" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="18"/>
+      <c r="A28" s="26"/>
       <c r="B28" s="9" t="s">
         <v>53</v>
       </c>
@@ -2089,7 +2146,7 @@
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="21" t="s">
+      <c r="H28" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I28" s="9"/>
@@ -2104,14 +2161,14 @@
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
       <c r="T28" s="9"/>
-      <c r="U28" s="21" t="s">
+      <c r="U28" s="19" t="s">
         <v>0</v>
       </c>
       <c r="V28" s="9"/>
-      <c r="W28" s="18"/>
+      <c r="W28" s="26"/>
     </row>
     <row r="29" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="26" t="s">
         <v>57</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -2119,12 +2176,12 @@
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="31" t="s">
         <v>67</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="21" t="s">
+      <c r="H29" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I29" s="9"/>
@@ -2141,25 +2198,25 @@
       <c r="R29" s="9"/>
       <c r="S29" s="9"/>
       <c r="T29" s="9"/>
-      <c r="U29" s="21" t="s">
+      <c r="U29" s="19" t="s">
         <v>0</v>
       </c>
       <c r="V29" s="9"/>
-      <c r="W29" s="18"/>
+      <c r="W29" s="26"/>
     </row>
     <row r="30" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="18"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="21" t="s">
+      <c r="H30" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I30" s="9"/>
@@ -2177,29 +2234,29 @@
       <c r="O30" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="P30" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q30" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="R30" s="11" t="s">
+      <c r="P30" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q30" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="R30" s="10" t="s">
         <v>62</v>
       </c>
       <c r="S30" s="11" t="s">
         <v>62</v>
       </c>
       <c r="T30" s="9"/>
-      <c r="U30" s="21" t="s">
+      <c r="U30" s="19" t="s">
         <v>0</v>
       </c>
       <c r="V30" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="W30" s="18"/>
+      <c r="W30" s="26"/>
     </row>
     <row r="31" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="18"/>
+      <c r="A31" s="26"/>
       <c r="B31" s="9" t="s">
         <v>50</v>
       </c>
@@ -2209,7 +2266,7 @@
       <c r="D31" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E31" s="21" t="s">
+      <c r="E31" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F31" s="10" t="s">
@@ -2218,7 +2275,7 @@
       <c r="G31" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H31" s="21" t="s">
+      <c r="H31" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I31" s="10" t="s">
@@ -2239,20 +2296,20 @@
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
+      <c r="Q31" s="10"/>
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
       <c r="T31" s="9"/>
-      <c r="U31" s="21" t="s">
+      <c r="U31" s="19" t="s">
         <v>0</v>
       </c>
       <c r="V31" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="W31" s="18"/>
+      <c r="W31" s="26"/>
     </row>
     <row r="32" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
+      <c r="A32" s="26"/>
       <c r="B32" s="9" t="s">
         <v>51</v>
       </c>
@@ -2262,7 +2319,7 @@
       <c r="D32" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E32" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F32" s="10" t="s">
@@ -2271,7 +2328,7 @@
       <c r="G32" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H32" s="21" t="s">
+      <c r="H32" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I32" s="10" t="s">
@@ -2296,27 +2353,27 @@
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
       <c r="T32" s="9"/>
-      <c r="U32" s="21" t="s">
+      <c r="U32" s="19" t="s">
         <v>0</v>
       </c>
       <c r="V32" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="W32" s="18"/>
+      <c r="W32" s="26"/>
     </row>
     <row r="33" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="18"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
-      <c r="E33" s="21" t="s">
+      <c r="E33" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="21" t="s">
+      <c r="H33" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I33" s="9"/>
@@ -2331,25 +2388,25 @@
       <c r="R33" s="9"/>
       <c r="S33" s="9"/>
       <c r="T33" s="9"/>
-      <c r="U33" s="21" t="s">
+      <c r="U33" s="19" t="s">
         <v>0</v>
       </c>
       <c r="V33" s="9"/>
-      <c r="W33" s="18"/>
+      <c r="W33" s="26"/>
     </row>
     <row r="34" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
-      <c r="E34" s="21" t="s">
+      <c r="E34" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="21" t="s">
+      <c r="H34" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I34" s="9"/>
@@ -2364,14 +2421,14 @@
       <c r="R34" s="9"/>
       <c r="S34" s="9"/>
       <c r="T34" s="9"/>
-      <c r="U34" s="21" t="s">
+      <c r="U34" s="19" t="s">
         <v>0</v>
       </c>
       <c r="V34" s="9"/>
-      <c r="W34" s="18"/>
+      <c r="W34" s="26"/>
     </row>
     <row r="35" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="26" t="s">
         <v>58</v>
       </c>
       <c r="B35" s="9" t="s">
@@ -2379,19 +2436,19 @@
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
-      <c r="E35" s="21" t="s">
+      <c r="E35" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
-      <c r="H35" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="I35" s="22" t="s">
+      <c r="H35" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="I35" s="21" t="s">
         <v>97</v>
       </c>
       <c r="J35" s="9"/>
-      <c r="K35" s="22" t="s">
+      <c r="K35" s="21" t="s">
         <v>97</v>
       </c>
       <c r="L35" s="9"/>
@@ -2400,66 +2457,66 @@
       <c r="O35" s="9"/>
       <c r="P35" s="9"/>
       <c r="Q35" s="9"/>
-      <c r="R35" s="27" t="s">
+      <c r="R35" s="21" t="s">
         <v>99</v>
       </c>
       <c r="S35" s="9"/>
       <c r="T35" s="9"/>
       <c r="U35" s="9"/>
       <c r="V35" s="9"/>
-      <c r="W35" s="18"/>
+      <c r="W35" s="26"/>
     </row>
     <row r="36" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="18"/>
+      <c r="A36" s="26"/>
       <c r="B36" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
-      <c r="E36" s="21" t="s">
+      <c r="E36" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
-      <c r="H36" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="I36" s="23"/>
+      <c r="H36" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="I36" s="22"/>
       <c r="J36" s="9"/>
-      <c r="K36" s="23"/>
+      <c r="K36" s="22"/>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
       <c r="O36" s="9"/>
       <c r="P36" s="9"/>
       <c r="Q36" s="9"/>
-      <c r="R36" s="28"/>
+      <c r="R36" s="22"/>
       <c r="S36" s="9"/>
       <c r="T36" s="9"/>
       <c r="U36" s="9"/>
       <c r="V36" s="9"/>
-      <c r="W36" s="18"/>
+      <c r="W36" s="26"/>
     </row>
     <row r="37" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="18"/>
+      <c r="A37" s="26"/>
       <c r="B37" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
-      <c r="E37" s="21" t="s">
+      <c r="E37" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
-      <c r="H37" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="I37" s="22" t="s">
+      <c r="H37" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" s="21" t="s">
         <v>95</v>
       </c>
       <c r="J37" s="9"/>
-      <c r="K37" s="22" t="s">
+      <c r="K37" s="21" t="s">
         <v>95</v>
       </c>
       <c r="L37" s="9"/>
@@ -2468,59 +2525,59 @@
       <c r="O37" s="9"/>
       <c r="P37" s="9"/>
       <c r="Q37" s="9"/>
-      <c r="R37" s="27" t="s">
+      <c r="R37" s="21" t="s">
         <v>100</v>
       </c>
       <c r="S37" s="9"/>
       <c r="T37" s="9"/>
       <c r="U37" s="9"/>
       <c r="V37" s="9"/>
-      <c r="W37" s="18"/>
+      <c r="W37" s="26"/>
     </row>
     <row r="38" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="18"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
-      <c r="E38" s="21" t="s">
+      <c r="E38" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
-      <c r="H38" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="I38" s="23"/>
+      <c r="H38" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="I38" s="22"/>
       <c r="J38" s="9"/>
-      <c r="K38" s="23"/>
+      <c r="K38" s="22"/>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
       <c r="Q38" s="9"/>
-      <c r="R38" s="28"/>
+      <c r="R38" s="22"/>
       <c r="S38" s="9"/>
       <c r="T38" s="9"/>
       <c r="U38" s="9"/>
       <c r="V38" s="9"/>
-      <c r="W38" s="18"/>
+      <c r="W38" s="26"/>
     </row>
     <row r="39" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="18"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
-      <c r="E39" s="21" t="s">
+      <c r="E39" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
-      <c r="H39" s="21" t="s">
+      <c r="H39" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I39" s="9"/>
@@ -2537,21 +2594,21 @@
       <c r="T39" s="9"/>
       <c r="U39" s="9"/>
       <c r="V39" s="9"/>
-      <c r="W39" s="18"/>
+      <c r="W39" s="26"/>
     </row>
     <row r="40" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="18"/>
+      <c r="A40" s="26"/>
       <c r="B40" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
-      <c r="E40" s="21" t="s">
+      <c r="E40" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
-      <c r="H40" s="21" t="s">
+      <c r="H40" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I40" s="9"/>
@@ -2568,10 +2625,10 @@
       <c r="T40" s="9"/>
       <c r="U40" s="9"/>
       <c r="V40" s="9"/>
-      <c r="W40" s="18"/>
+      <c r="W40" s="26"/>
     </row>
     <row r="41" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="18" t="s">
+      <c r="A41" s="26" t="s">
         <v>59</v>
       </c>
       <c r="B41" s="9" t="s">
@@ -2579,12 +2636,12 @@
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
-      <c r="E41" s="21" t="s">
+      <c r="E41" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
-      <c r="H41" s="21" t="s">
+      <c r="H41" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I41" s="9"/>
@@ -2596,28 +2653,30 @@
       <c r="O41" s="9"/>
       <c r="P41" s="9"/>
       <c r="Q41" s="9"/>
-      <c r="R41" s="9"/>
+      <c r="R41" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="S41" s="9"/>
       <c r="T41" s="9"/>
       <c r="U41" s="9"/>
       <c r="V41" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="W41" s="18"/>
+      <c r="W41" s="26"/>
     </row>
     <row r="42" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="18"/>
+      <c r="A42" s="26"/>
       <c r="B42" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
-      <c r="E42" s="21" t="s">
+      <c r="E42" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I42" s="9"/>
@@ -2629,28 +2688,30 @@
       <c r="O42" s="9"/>
       <c r="P42" s="9"/>
       <c r="Q42" s="9"/>
-      <c r="R42" s="9"/>
+      <c r="R42" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="S42" s="9"/>
       <c r="T42" s="9"/>
       <c r="U42" s="9"/>
       <c r="V42" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="W42" s="18"/>
+      <c r="W42" s="26"/>
     </row>
     <row r="43" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="18"/>
+      <c r="A43" s="26"/>
       <c r="B43" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
-      <c r="E43" s="21" t="s">
+      <c r="E43" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I43" s="9"/>
@@ -2662,28 +2723,30 @@
       <c r="O43" s="9"/>
       <c r="P43" s="9"/>
       <c r="Q43" s="9"/>
-      <c r="R43" s="9"/>
+      <c r="R43" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="S43" s="9"/>
       <c r="T43" s="9"/>
       <c r="U43" s="9"/>
       <c r="V43" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="W43" s="18"/>
+      <c r="W43" s="26"/>
     </row>
     <row r="44" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="18"/>
+      <c r="A44" s="26"/>
       <c r="B44" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
-      <c r="E44" s="21" t="s">
+      <c r="E44" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
-      <c r="H44" s="21" t="s">
+      <c r="H44" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I44" s="9"/>
@@ -2695,28 +2758,30 @@
       <c r="O44" s="9"/>
       <c r="P44" s="9"/>
       <c r="Q44" s="9"/>
-      <c r="R44" s="9"/>
+      <c r="R44" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="S44" s="9"/>
       <c r="T44" s="9"/>
       <c r="U44" s="9"/>
       <c r="V44" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="W44" s="18"/>
+      <c r="W44" s="26"/>
     </row>
     <row r="45" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="18"/>
+      <c r="A45" s="26"/>
       <c r="B45" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
-      <c r="E45" s="21" t="s">
+      <c r="E45" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
-      <c r="H45" s="21" t="s">
+      <c r="H45" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I45" s="9"/>
@@ -2728,28 +2793,30 @@
       <c r="O45" s="9"/>
       <c r="P45" s="9"/>
       <c r="Q45" s="9"/>
-      <c r="R45" s="9"/>
+      <c r="R45" s="10" t="s">
+        <v>105</v>
+      </c>
       <c r="S45" s="9"/>
       <c r="T45" s="9"/>
       <c r="U45" s="9"/>
       <c r="V45" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="W45" s="18"/>
+      <c r="W45" s="26"/>
     </row>
     <row r="46" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
+      <c r="A46" s="26"/>
       <c r="B46" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
-      <c r="E46" s="21" t="s">
+      <c r="E46" s="31" t="s">
         <v>0</v>
       </c>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
-      <c r="H46" s="21" t="s">
+      <c r="H46" s="31" t="s">
         <v>0</v>
       </c>
       <c r="I46" s="9"/>
@@ -2766,60 +2833,69 @@
       <c r="T46" s="9"/>
       <c r="U46" s="9"/>
       <c r="V46" s="9"/>
-      <c r="W46" s="18"/>
+      <c r="W46" s="26"/>
     </row>
     <row r="47" spans="1:23" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18"/>
-      <c r="M47" s="18"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
-      <c r="T47" s="18"/>
-      <c r="U47" s="18"/>
-      <c r="V47" s="18"/>
-      <c r="W47" s="18"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="26"/>
+      <c r="L47" s="26"/>
+      <c r="M47" s="26"/>
+      <c r="N47" s="26"/>
+      <c r="O47" s="26"/>
+      <c r="P47" s="26"/>
+      <c r="Q47" s="26"/>
+      <c r="R47" s="26"/>
+      <c r="S47" s="26"/>
+      <c r="T47" s="26"/>
+      <c r="U47" s="26"/>
+      <c r="V47" s="26"/>
+      <c r="W47" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="R35:R36"/>
-    <mergeCell ref="R37:R38"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="Q13:Q14"/>
+  <mergeCells count="60">
+    <mergeCell ref="U25:U26"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A35:A40"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="I25:I26"/>
     <mergeCell ref="I37:I38"/>
     <mergeCell ref="K37:K38"/>
     <mergeCell ref="I35:I36"/>
     <mergeCell ref="K35:K36"/>
+    <mergeCell ref="U17:U21"/>
     <mergeCell ref="L26:L27"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="R35:R36"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="A47:W47"/>
+    <mergeCell ref="W5:W46"/>
+    <mergeCell ref="E29:E46"/>
+    <mergeCell ref="H11:H46"/>
+    <mergeCell ref="I5:I10"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="U5:U6"/>
     <mergeCell ref="A1:W1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="M2:W2"/>
@@ -2832,28 +2908,22 @@
     <mergeCell ref="N15:N16"/>
     <mergeCell ref="M14:M15"/>
     <mergeCell ref="M8:M9"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="L21:L22"/>
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="L15:L16"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="A35:A40"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="A47:W47"/>
-    <mergeCell ref="W5:W46"/>
-    <mergeCell ref="U17:U34"/>
-    <mergeCell ref="E29:E46"/>
-    <mergeCell ref="H11:H46"/>
-    <mergeCell ref="I5:I10"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="R37:R38"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="R13:R14"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>